<commit_message>
testcase: add temp find merchandise
</commit_message>
<xml_diff>
--- a/Testcase/03-Testcase-1.xlsx
+++ b/Testcase/03-Testcase-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SE\HKI VII\tesing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buiqu\OneDrive\Documents\GitHub\OnlineShop\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7188ACA-42F4-496E-BC74-745E3126AD41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05B479F-BFCD-40DA-919F-048D25743232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="794" firstSheet="6" activeTab="10" xr2:uid="{DF3F47F0-DBD9-4663-B187-A3CC9925D78A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="794" firstSheet="6" activeTab="11" xr2:uid="{DF3F47F0-DBD9-4663-B187-A3CC9925D78A}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="301">
   <si>
     <t>UNIT TEST CASE</t>
   </si>
@@ -1428,6 +1428,18 @@
   </si>
   <si>
     <t>"456"</t>
+  </si>
+  <si>
+    <t>Giao diện quản lí account được mở</t>
+  </si>
+  <si>
+    <t>Giao diện tìm kiếm được mở</t>
+  </si>
+  <si>
+    <t>Text search</t>
+  </si>
+  <si>
+    <t>list count = 28</t>
   </si>
 </sst>
 </file>
@@ -3664,6 +3676,102 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="40" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="42" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="57" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="26" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3718,101 +3826,11 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="64" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="65" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="40" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="42" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="57" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="26" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3844,12 +3862,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="64" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="65" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3934,9 +3946,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="103" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3944,6 +3953,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4897,43 +4909,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="245" t="str">
+      <c r="B1" s="264"/>
+      <c r="C1" s="277" t="str">
         <f>FunctionList!E14</f>
         <v>FN04</v>
       </c>
-      <c r="D1" s="246"/>
+      <c r="D1" s="278"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D14</f>
         <v>Sửa tài khoản</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="236"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
       <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -4960,10 +4972,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -4991,82 +5003,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F68:HJ68,"P")</f>
         <v>0</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F68:HJ68,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E66:HJ66,"N")</f>
         <v>0</v>
@@ -5079,15 +5091,15 @@
         <f>COUNTIF(E66:HJ66,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HM8)</f>
         <v>9</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1"/>
     <row r="8" spans="1:21" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -5306,10 +5318,10 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="276" t="s">
+      <c r="D18" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="276"/>
+      <c r="E18" s="231"/>
       <c r="F18" s="110" t="s">
         <v>101</v>
       </c>
@@ -5395,7 +5407,7 @@
       <c r="A22" s="78"/>
       <c r="B22" s="79"/>
       <c r="C22" s="80"/>
-      <c r="D22" s="276" t="s">
+      <c r="D22" s="231" t="s">
         <v>81</v>
       </c>
       <c r="E22" s="320"/>
@@ -5467,10 +5479,10 @@
       <c r="A25" s="78"/>
       <c r="B25" s="79"/>
       <c r="C25" s="80"/>
-      <c r="D25" s="276" t="s">
+      <c r="D25" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="276"/>
+      <c r="E25" s="231"/>
       <c r="F25" s="110" t="s">
         <v>101</v>
       </c>
@@ -6671,14 +6683,11 @@
     <row r="77" spans="1:14" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:K6"/>
     <mergeCell ref="O6:T6"/>
     <mergeCell ref="A3:B3"/>
@@ -6692,11 +6701,14 @@
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:T5"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I18 F18:H19 M9:M19 F9:L17 J18:L19 N9:N72 F20:M72" xr:uid="{F5D02F7C-4E5B-408B-A811-49F480D78479}">
@@ -6719,7 +6731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B58DD7-DF61-434E-B1F4-345EEB1D4501}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
@@ -6742,35 +6754,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="245" t="str">
+      <c r="B1" s="264"/>
+      <c r="C1" s="277" t="str">
         <f>FunctionList!E14</f>
         <v>FN04</v>
       </c>
-      <c r="D1" s="246"/>
+      <c r="D1" s="278"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="235"/>
-      <c r="K1" s="235"/>
-      <c r="L1" s="235"/>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="236"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="268"/>
       <c r="P1" s="119"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -6790,10 +6802,10 @@
       <c r="O2" s="64"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -6813,77 +6825,77 @@
       <c r="O3" s="298"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="274"/>
-      <c r="K4" s="274"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="246"/>
+      <c r="K4" s="246"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="249" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="250"/>
-      <c r="L5" s="250"/>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="251"/>
+      <c r="K5" s="249"/>
+      <c r="L5" s="249"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="250"/>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F68:HE68,"P")</f>
         <v>0</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F68:HE68,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(J6,- A6,- C6)</f>
         <v>4</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="257">
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="256">
         <f>COUNTA(E8:HH8)</f>
         <v>4</v>
       </c>
-      <c r="K6" s="255"/>
-      <c r="L6" s="255"/>
-      <c r="M6" s="255"/>
-      <c r="N6" s="255"/>
-      <c r="O6" s="258"/>
+      <c r="K6" s="254"/>
+      <c r="L6" s="254"/>
+      <c r="M6" s="254"/>
+      <c r="N6" s="254"/>
+      <c r="O6" s="257"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1"/>
     <row r="8" spans="1:16" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -7032,10 +7044,10 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="276" t="s">
+      <c r="D18" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="276"/>
+      <c r="E18" s="231"/>
       <c r="F18" s="110" t="s">
         <v>101</v>
       </c>
@@ -7109,7 +7121,7 @@
       <c r="A23" s="78"/>
       <c r="B23" s="79"/>
       <c r="C23" s="80"/>
-      <c r="D23" s="276" t="s">
+      <c r="D23" s="231" t="s">
         <v>81</v>
       </c>
       <c r="E23" s="320"/>
@@ -7152,10 +7164,10 @@
       <c r="A26" s="78"/>
       <c r="B26" s="79"/>
       <c r="C26" s="80"/>
-      <c r="D26" s="276" t="s">
+      <c r="D26" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="276"/>
+      <c r="E26" s="231"/>
       <c r="F26" s="110" t="s">
         <v>101</v>
       </c>
@@ -7929,23 +7941,6 @@
     <row r="77" spans="1:9" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:O4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:I1"/>
@@ -7953,6 +7948,23 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F73:I73" xr:uid="{39298C94-86F9-45D3-AB0D-ACA88CABDB5F}">
@@ -7975,8 +7987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5165FA15-CC46-40B0-8B50-C77CFB285AC3}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8003,43 +8015,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="281"/>
+      <c r="B1" s="283"/>
       <c r="C1" s="302" t="str">
         <f>FunctionList!E13</f>
         <v>FN03</v>
       </c>
-      <c r="D1" s="288"/>
+      <c r="D1" s="290"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D13</f>
         <v>Thêm mới tài khoản</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="236"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
       <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>65</v>
       </c>
@@ -8064,10 +8076,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -8095,82 +8107,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F51:HE51,"P")</f>
         <v>3</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F51:HE51,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E50:HE50,"N")</f>
         <v>3</v>
@@ -8183,15 +8195,15 @@
         <f>COUNTIF(E50:HE50,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HH8)</f>
         <v>3</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1"/>
     <row r="8" spans="1:21" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -8240,7 +8252,9 @@
       <c r="A11" s="78"/>
       <c r="B11" s="79"/>
       <c r="C11" s="80"/>
-      <c r="D11" s="81"/>
+      <c r="D11" s="81" t="s">
+        <v>298</v>
+      </c>
       <c r="E11" s="76"/>
       <c r="F11" s="110"/>
       <c r="G11" s="110"/>
@@ -8259,7 +8273,7 @@
     <row r="13" spans="1:21">
       <c r="A13" s="78"/>
       <c r="B13" s="79" t="s">
-        <v>97</v>
+        <v>299</v>
       </c>
       <c r="C13" s="80"/>
       <c r="D13" s="81"/>
@@ -8291,9 +8305,7 @@
       </c>
       <c r="E15" s="84"/>
       <c r="F15" s="110"/>
-      <c r="G15" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G15" s="110"/>
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:21">
@@ -8306,15 +8318,11 @@
       <c r="E16" s="84"/>
       <c r="F16" s="110"/>
       <c r="G16" s="110"/>
-      <c r="H16" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="H16" s="110"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="78"/>
-      <c r="B17" s="79" t="s">
-        <v>197</v>
-      </c>
+      <c r="B17" s="79"/>
       <c r="C17" s="80"/>
       <c r="D17" s="81"/>
       <c r="E17" s="84"/>
@@ -8326,13 +8334,9 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="81" t="s">
-        <v>81</v>
-      </c>
+      <c r="D18" s="81"/>
       <c r="E18" s="84"/>
-      <c r="F18" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F18" s="110"/>
       <c r="G18" s="110"/>
       <c r="H18" s="110"/>
     </row>
@@ -8340,23 +8344,15 @@
       <c r="A19" s="78"/>
       <c r="B19" s="79"/>
       <c r="C19" s="80"/>
-      <c r="D19" s="81" t="s">
-        <v>223</v>
-      </c>
+      <c r="D19" s="81"/>
       <c r="E19" s="84"/>
       <c r="F19" s="110"/>
-      <c r="G19" s="110" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="78"/>
-      <c r="B20" s="79" t="s">
-        <v>198</v>
-      </c>
+      <c r="B20" s="79"/>
       <c r="C20" s="80"/>
       <c r="D20" s="81"/>
       <c r="E20" s="84"/>
@@ -8368,13 +8364,9 @@
       <c r="A21" s="78"/>
       <c r="B21" s="79"/>
       <c r="C21" s="80"/>
-      <c r="D21" s="81" t="s">
-        <v>81</v>
-      </c>
+      <c r="D21" s="81"/>
       <c r="E21" s="84"/>
-      <c r="F21" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F21" s="110"/>
       <c r="G21" s="110"/>
       <c r="H21" s="110"/>
     </row>
@@ -8382,23 +8374,15 @@
       <c r="A22" s="78"/>
       <c r="B22" s="79"/>
       <c r="C22" s="80"/>
-      <c r="D22" s="81" t="s">
-        <v>202</v>
-      </c>
+      <c r="D22" s="81"/>
       <c r="E22" s="84"/>
       <c r="F22" s="110"/>
-      <c r="G22" s="110" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="78"/>
-      <c r="B23" s="79" t="s">
-        <v>199</v>
-      </c>
+      <c r="B23" s="79"/>
       <c r="C23" s="80"/>
       <c r="D23" s="81"/>
       <c r="E23" s="84"/>
@@ -8410,13 +8394,9 @@
       <c r="A24" s="78"/>
       <c r="B24" s="79"/>
       <c r="C24" s="80"/>
-      <c r="D24" s="188" t="s">
-        <v>81</v>
-      </c>
+      <c r="D24" s="188"/>
       <c r="E24" s="84"/>
-      <c r="F24" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F24" s="110"/>
       <c r="G24" s="110"/>
       <c r="H24" s="110"/>
     </row>
@@ -8424,23 +8404,15 @@
       <c r="A25" s="78"/>
       <c r="B25" s="79"/>
       <c r="C25" s="80"/>
-      <c r="D25" s="81" t="s">
-        <v>226</v>
-      </c>
+      <c r="D25" s="81"/>
       <c r="E25" s="84"/>
       <c r="F25" s="110"/>
-      <c r="G25" s="110" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="78"/>
-      <c r="B26" s="79" t="s">
-        <v>230</v>
-      </c>
+      <c r="B26" s="79"/>
       <c r="C26" s="80"/>
       <c r="D26" s="81"/>
       <c r="E26" s="84"/>
@@ -8452,13 +8424,9 @@
       <c r="A27" s="78"/>
       <c r="B27" s="79"/>
       <c r="C27" s="80"/>
-      <c r="D27" s="81" t="s">
-        <v>81</v>
-      </c>
+      <c r="D27" s="81"/>
       <c r="E27" s="84"/>
-      <c r="F27" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F27" s="110"/>
       <c r="G27" s="110"/>
       <c r="H27" s="110"/>
     </row>
@@ -8466,23 +8434,15 @@
       <c r="A28" s="78"/>
       <c r="B28" s="79"/>
       <c r="C28" s="80"/>
-      <c r="D28" s="81" t="s">
-        <v>234</v>
-      </c>
+      <c r="D28" s="81"/>
       <c r="E28" s="84"/>
       <c r="F28" s="110"/>
-      <c r="G28" s="110" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="78"/>
-      <c r="B29" s="79" t="s">
-        <v>231</v>
-      </c>
+      <c r="B29" s="79"/>
       <c r="C29" s="80"/>
       <c r="D29" s="81"/>
       <c r="E29" s="84"/>
@@ -8494,13 +8454,9 @@
       <c r="A30" s="78"/>
       <c r="B30" s="79"/>
       <c r="C30" s="80"/>
-      <c r="D30" s="81" t="s">
-        <v>81</v>
-      </c>
+      <c r="D30" s="81"/>
       <c r="E30" s="84"/>
-      <c r="F30" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F30" s="110"/>
       <c r="G30" s="110"/>
       <c r="H30" s="110"/>
     </row>
@@ -8508,35 +8464,25 @@
       <c r="A31" s="78"/>
       <c r="B31" s="79"/>
       <c r="C31" s="80"/>
-      <c r="D31" s="81" t="s">
-        <v>236</v>
-      </c>
+      <c r="D31" s="81"/>
       <c r="E31" s="84"/>
       <c r="F31" s="110"/>
       <c r="G31" s="110"/>
-      <c r="H31" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="H31" s="110"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="78"/>
       <c r="B32" s="79"/>
       <c r="C32" s="80"/>
-      <c r="D32" s="81" t="s">
-        <v>235</v>
-      </c>
+      <c r="D32" s="81"/>
       <c r="E32" s="84"/>
       <c r="F32" s="110"/>
-      <c r="G32" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G32" s="110"/>
       <c r="H32" s="110"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="78"/>
-      <c r="B33" s="79" t="s">
-        <v>232</v>
-      </c>
+      <c r="B33" s="79"/>
       <c r="C33" s="80"/>
       <c r="D33" s="81"/>
       <c r="E33" s="84"/>
@@ -8548,39 +8494,27 @@
       <c r="A34" s="78"/>
       <c r="B34" s="79"/>
       <c r="C34" s="80"/>
-      <c r="D34" s="81" t="s">
-        <v>81</v>
-      </c>
+      <c r="D34" s="81"/>
       <c r="E34" s="84"/>
-      <c r="F34" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F34" s="110"/>
       <c r="G34" s="110"/>
-      <c r="H34" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="H34" s="110"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="78"/>
       <c r="B35" s="79"/>
       <c r="C35" s="80"/>
-      <c r="D35" s="81" t="s">
-        <v>237</v>
-      </c>
+      <c r="D35" s="81"/>
       <c r="E35" s="84"/>
       <c r="F35" s="110"/>
-      <c r="G35" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G35" s="110"/>
       <c r="H35" s="110"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="78"/>
       <c r="B36" s="132"/>
       <c r="C36" s="133"/>
-      <c r="D36" s="134" t="s">
-        <v>238</v>
-      </c>
+      <c r="D36" s="134"/>
       <c r="E36" s="84"/>
       <c r="F36" s="128"/>
       <c r="G36" s="128"/>
@@ -8590,9 +8524,7 @@
       <c r="A37" s="78"/>
       <c r="B37" s="132"/>
       <c r="C37" s="133"/>
-      <c r="D37" s="134" t="s">
-        <v>239</v>
-      </c>
+      <c r="D37" s="134"/>
       <c r="E37" s="84"/>
       <c r="F37" s="128"/>
       <c r="G37" s="128"/>
@@ -8602,9 +8534,7 @@
       <c r="A38" s="78"/>
       <c r="B38" s="85"/>
       <c r="C38" s="86"/>
-      <c r="D38" s="87" t="s">
-        <v>240</v>
-      </c>
+      <c r="D38" s="87"/>
       <c r="E38" s="88"/>
       <c r="F38" s="129"/>
       <c r="G38" s="129"/>
@@ -8629,13 +8559,13 @@
       <c r="B40" s="96"/>
       <c r="C40" s="97"/>
       <c r="D40" s="98" t="s">
-        <v>114</v>
+        <v>300</v>
       </c>
       <c r="E40" s="99"/>
-      <c r="F40" s="110"/>
-      <c r="G40" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F40" s="110" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="110"/>
       <c r="H40" s="110"/>
     </row>
     <row r="41" spans="1:8">
@@ -8648,9 +8578,7 @@
       <c r="E41" s="99"/>
       <c r="F41" s="110"/>
       <c r="G41" s="110"/>
-      <c r="H41" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="H41" s="110"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="95"/>
@@ -8684,9 +8612,7 @@
         <v>243</v>
       </c>
       <c r="E44" s="101"/>
-      <c r="F44" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="F44" s="110"/>
       <c r="G44" s="110"/>
       <c r="H44" s="110"/>
     </row>
@@ -8728,14 +8654,10 @@
       <c r="A48" s="95"/>
       <c r="B48" s="96"/>
       <c r="C48" s="100"/>
-      <c r="D48" s="98" t="s">
-        <v>244</v>
-      </c>
+      <c r="D48" s="98"/>
       <c r="E48" s="101"/>
       <c r="F48" s="110"/>
-      <c r="G48" s="110" t="s">
-        <v>101</v>
-      </c>
+      <c r="G48" s="110"/>
       <c r="H48" s="110"/>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1">
@@ -8752,11 +8674,11 @@
       <c r="A50" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="277" t="s">
+      <c r="B50" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="277"/>
-      <c r="D50" s="277"/>
+      <c r="C50" s="232"/>
+      <c r="D50" s="232"/>
       <c r="E50" s="187"/>
       <c r="F50" s="108" t="s">
         <v>53</v>
@@ -8770,11 +8692,11 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="95"/>
-      <c r="B51" s="278" t="s">
+      <c r="B51" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="278"/>
-      <c r="D51" s="278"/>
+      <c r="C51" s="233"/>
+      <c r="D51" s="233"/>
       <c r="E51" s="109"/>
       <c r="F51" s="110" t="s">
         <v>91</v>
@@ -8788,11 +8710,11 @@
     </row>
     <row r="52" spans="1:8" ht="13.5" customHeight="1">
       <c r="A52" s="95"/>
-      <c r="B52" s="279" t="s">
+      <c r="B52" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="279"/>
-      <c r="D52" s="279"/>
+      <c r="C52" s="234"/>
+      <c r="D52" s="234"/>
       <c r="E52" s="111"/>
       <c r="F52" s="112">
         <v>43468</v>
@@ -8806,11 +8728,11 @@
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1">
       <c r="A53" s="113"/>
-      <c r="B53" s="280" t="s">
+      <c r="B53" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="280"/>
-      <c r="D53" s="280"/>
+      <c r="C53" s="235"/>
+      <c r="D53" s="235"/>
       <c r="E53" s="114"/>
       <c r="F53" s="115"/>
       <c r="G53" s="115"/>
@@ -8819,25 +8741,6 @@
     <row r="54" spans="1:8" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="L3:T3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:T4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:K1"/>
@@ -8846,6 +8749,25 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:T4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:H49" xr:uid="{3DC1F670-276C-411B-9F94-F225DA618B2F}">
@@ -8895,42 +8817,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="264"/>
       <c r="C1" s="302" t="str">
         <f>FunctionList!E17</f>
         <v>FN07</v>
       </c>
-      <c r="D1" s="288"/>
+      <c r="D1" s="290"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D17</f>
         <v>Thêm danh mục sản phẩm</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="282"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="284"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -8944,9 +8866,9 @@
       <c r="I2" s="294"/>
       <c r="J2" s="294"/>
       <c r="K2" s="295"/>
-      <c r="L2" s="321"/>
-      <c r="M2" s="321"/>
-      <c r="N2" s="321"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="324"/>
+      <c r="N2" s="324"/>
       <c r="O2" s="120"/>
       <c r="P2" s="120"/>
       <c r="Q2" s="120"/>
@@ -8955,11 +8877,11 @@
       <c r="T2" s="121"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
-      <c r="C3" s="322">
+      <c r="B3" s="237"/>
+      <c r="C3" s="321">
         <v>100</v>
       </c>
       <c r="D3" s="297"/>
@@ -8986,82 +8908,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="323"/>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="324"/>
-      <c r="G4" s="324"/>
-      <c r="H4" s="324"/>
-      <c r="I4" s="324"/>
-      <c r="J4" s="324"/>
-      <c r="K4" s="324"/>
-      <c r="L4" s="323"/>
-      <c r="M4" s="323"/>
-      <c r="N4" s="323"/>
-      <c r="O4" s="323"/>
-      <c r="P4" s="323"/>
-      <c r="Q4" s="323"/>
-      <c r="R4" s="323"/>
-      <c r="S4" s="323"/>
-      <c r="T4" s="323"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="322"/>
+      <c r="D4" s="322"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="323"/>
+      <c r="G4" s="323"/>
+      <c r="H4" s="323"/>
+      <c r="I4" s="323"/>
+      <c r="J4" s="323"/>
+      <c r="K4" s="323"/>
+      <c r="L4" s="322"/>
+      <c r="M4" s="322"/>
+      <c r="N4" s="322"/>
+      <c r="O4" s="322"/>
+      <c r="P4" s="322"/>
+      <c r="Q4" s="322"/>
+      <c r="R4" s="322"/>
+      <c r="S4" s="322"/>
+      <c r="T4" s="322"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F31:HF31,"P")</f>
         <v>4</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F31:HF31,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E30:HF30,"N")</f>
         <v>4</v>
@@ -9074,15 +8996,15 @@
         <f>COUNTIF(E30:HF30,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HI8)</f>
         <v>4</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1"/>
     <row r="8" spans="1:20" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -9229,10 +9151,10 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="276" t="s">
+      <c r="D18" s="231" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="276"/>
+      <c r="E18" s="231"/>
       <c r="F18" s="110" t="s">
         <v>101</v>
       </c>
@@ -9395,11 +9317,11 @@
       <c r="A30" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="277" t="s">
+      <c r="B30" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="277"/>
-      <c r="D30" s="277"/>
+      <c r="C30" s="232"/>
+      <c r="D30" s="232"/>
       <c r="E30" s="107"/>
       <c r="F30" s="108" t="s">
         <v>53</v>
@@ -9416,11 +9338,11 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="95"/>
-      <c r="B31" s="278" t="s">
+      <c r="B31" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="278"/>
-      <c r="D31" s="278"/>
+      <c r="C31" s="233"/>
+      <c r="D31" s="233"/>
       <c r="E31" s="109"/>
       <c r="F31" s="110" t="s">
         <v>91</v>
@@ -9437,11 +9359,11 @@
     </row>
     <row r="32" spans="1:9" ht="14.25" customHeight="1">
       <c r="A32" s="95"/>
-      <c r="B32" s="279" t="s">
+      <c r="B32" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="279"/>
-      <c r="D32" s="279"/>
+      <c r="C32" s="234"/>
+      <c r="D32" s="234"/>
       <c r="E32" s="111"/>
       <c r="F32" s="112">
         <v>43468</v>
@@ -9458,11 +9380,11 @@
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1">
       <c r="A33" s="113"/>
-      <c r="B33" s="280" t="s">
+      <c r="B33" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="280"/>
-      <c r="D33" s="280"/>
+      <c r="C33" s="235"/>
+      <c r="D33" s="235"/>
       <c r="E33" s="114"/>
       <c r="F33" s="115"/>
       <c r="G33" s="115"/>
@@ -9472,11 +9394,13 @@
     <row r="34" spans="1:9" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
@@ -9493,13 +9417,11 @@
     <mergeCell ref="L1:T1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F30:I30" xr:uid="{20B68117-7AD7-4F54-8A55-B2FB1DCA6A99}">
@@ -9522,7 +9444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7FAAC0-1672-4B1E-87F9-0B635B04E116}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -9550,42 +9472,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="264"/>
       <c r="C1" s="302" t="str">
         <f>FunctionList!E18</f>
         <v>FN08</v>
       </c>
-      <c r="D1" s="288"/>
+      <c r="D1" s="290"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D18</f>
         <v>Sửa danh mục sản phẩm</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="282"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="284"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -9610,10 +9532,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -9641,82 +9563,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F35:HF35,"P")</f>
         <v>4</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F35:HF35,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E34:HF34,"N")</f>
         <v>4</v>
@@ -9729,15 +9651,15 @@
         <f>COUNTIF(E34:HF34,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HI8)</f>
         <v>4</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1"/>
     <row r="8" spans="1:20" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -9884,10 +9806,10 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="276">
+      <c r="D18" s="231">
         <v>0.5</v>
       </c>
-      <c r="E18" s="276"/>
+      <c r="E18" s="231"/>
       <c r="F18" s="110" t="s">
         <v>101</v>
       </c>
@@ -10118,11 +10040,11 @@
       <c r="A34" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="277" t="s">
+      <c r="B34" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="277"/>
-      <c r="D34" s="277"/>
+      <c r="C34" s="232"/>
+      <c r="D34" s="232"/>
       <c r="E34" s="107"/>
       <c r="F34" s="108" t="s">
         <v>53</v>
@@ -10139,11 +10061,11 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="95"/>
-      <c r="B35" s="278" t="s">
+      <c r="B35" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="278"/>
-      <c r="D35" s="278"/>
+      <c r="C35" s="233"/>
+      <c r="D35" s="233"/>
       <c r="E35" s="109"/>
       <c r="F35" s="110" t="s">
         <v>91</v>
@@ -10160,11 +10082,11 @@
     </row>
     <row r="36" spans="1:9" ht="13.5" customHeight="1">
       <c r="A36" s="95"/>
-      <c r="B36" s="279" t="s">
+      <c r="B36" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="279"/>
-      <c r="D36" s="279"/>
+      <c r="C36" s="234"/>
+      <c r="D36" s="234"/>
       <c r="E36" s="111"/>
       <c r="F36" s="112">
         <v>43468</v>
@@ -10181,11 +10103,11 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1">
       <c r="A37" s="113"/>
-      <c r="B37" s="280" t="s">
+      <c r="B37" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="280"/>
-      <c r="D37" s="280"/>
+      <c r="C37" s="235"/>
+      <c r="D37" s="235"/>
       <c r="E37" s="114"/>
       <c r="F37" s="115"/>
       <c r="G37" s="115"/>
@@ -10195,11 +10117,13 @@
     <row r="38" spans="1:9" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
@@ -10216,13 +10140,11 @@
     <mergeCell ref="L1:T1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:I34" xr:uid="{67BC5341-41C0-477A-8962-FFFAE5337B7D}">
@@ -10244,8 +10166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AFDBDC-9AA8-4DC5-8DC6-1A9F5F7869F5}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11017,7 +10939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9464DEA-5289-45F9-A9DC-72A5F42A6A60}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -11627,176 +11549,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="245" t="str">
+      <c r="B1" s="264"/>
+      <c r="C1" s="277" t="str">
         <f>FunctionList!E11</f>
         <v>FN01</v>
       </c>
-      <c r="D1" s="246"/>
+      <c r="D1" s="278"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D11</f>
         <v>Đăng nhập</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="236"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
       <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="269" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="247" t="s">
+      <c r="B2" s="270"/>
+      <c r="C2" s="279" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="248"/>
+      <c r="D2" s="280"/>
       <c r="E2" s="118"/>
-      <c r="F2" s="239" t="s">
+      <c r="F2" s="271" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="240"/>
-      <c r="H2" s="240"/>
-      <c r="I2" s="240"/>
-      <c r="J2" s="240"/>
-      <c r="K2" s="241"/>
-      <c r="L2" s="242" t="s">
+      <c r="G2" s="272"/>
+      <c r="H2" s="272"/>
+      <c r="I2" s="272"/>
+      <c r="J2" s="272"/>
+      <c r="K2" s="273"/>
+      <c r="L2" s="274" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="243"/>
-      <c r="N2" s="243"/>
-      <c r="O2" s="243"/>
-      <c r="P2" s="243"/>
-      <c r="Q2" s="243"/>
-      <c r="R2" s="243"/>
-      <c r="S2" s="243"/>
-      <c r="T2" s="244"/>
+      <c r="M2" s="275"/>
+      <c r="N2" s="275"/>
+      <c r="O2" s="275"/>
+      <c r="P2" s="275"/>
+      <c r="Q2" s="275"/>
+      <c r="R2" s="275"/>
+      <c r="S2" s="275"/>
+      <c r="T2" s="276"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
-      <c r="C3" s="266">
+      <c r="B3" s="237"/>
+      <c r="C3" s="238">
         <v>100</v>
       </c>
-      <c r="D3" s="267"/>
+      <c r="D3" s="239"/>
       <c r="E3" s="65"/>
-      <c r="F3" s="268" t="s">
+      <c r="F3" s="240" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="269"/>
-      <c r="H3" s="269"/>
-      <c r="I3" s="269"/>
-      <c r="J3" s="269"/>
-      <c r="K3" s="270"/>
-      <c r="L3" s="271">
+      <c r="G3" s="241"/>
+      <c r="H3" s="241"/>
+      <c r="I3" s="241"/>
+      <c r="J3" s="241"/>
+      <c r="K3" s="242"/>
+      <c r="L3" s="243">
         <f xml:space="preserve"> IF(FunctionList!E6&lt;&gt;"N/A",SUM(C3*FunctionList!E6/1000,- O6),"N/A")</f>
         <v>2</v>
       </c>
-      <c r="M3" s="272"/>
-      <c r="N3" s="272"/>
-      <c r="O3" s="272"/>
-      <c r="P3" s="272"/>
-      <c r="Q3" s="272"/>
-      <c r="R3" s="272"/>
-      <c r="S3" s="272"/>
-      <c r="T3" s="273"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="244"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="245"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F38:HQ38,"P")</f>
         <v>8</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F38:HQ38,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E37:HJ37,"N")</f>
         <v>8</v>
@@ -11809,15 +11731,15 @@
         <f>COUNTIF(E37:HJ37,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HM8)</f>
         <v>8</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1"/>
     <row r="8" spans="1:21" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -12005,10 +11927,10 @@
       <c r="A17" s="78"/>
       <c r="B17" s="79"/>
       <c r="C17" s="80"/>
-      <c r="D17" s="276" t="s">
+      <c r="D17" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="276"/>
+      <c r="E17" s="231"/>
       <c r="F17" s="110" t="s">
         <v>101</v>
       </c>
@@ -12377,11 +12299,11 @@
       <c r="A37" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="277" t="s">
+      <c r="B37" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="277"/>
-      <c r="D37" s="277"/>
+      <c r="C37" s="232"/>
+      <c r="D37" s="232"/>
       <c r="E37" s="107"/>
       <c r="F37" s="108" t="s">
         <v>53</v>
@@ -12410,11 +12332,11 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="95"/>
-      <c r="B38" s="278" t="s">
+      <c r="B38" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="278"/>
-      <c r="D38" s="278"/>
+      <c r="C38" s="233"/>
+      <c r="D38" s="233"/>
       <c r="E38" s="109"/>
       <c r="F38" s="110" t="s">
         <v>91</v>
@@ -12443,11 +12365,11 @@
     </row>
     <row r="39" spans="1:13" ht="12.75" customHeight="1">
       <c r="A39" s="95"/>
-      <c r="B39" s="279" t="s">
+      <c r="B39" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="279"/>
-      <c r="D39" s="279"/>
+      <c r="C39" s="234"/>
+      <c r="D39" s="234"/>
       <c r="E39" s="111"/>
       <c r="F39" s="123">
         <v>43467</v>
@@ -12476,11 +12398,11 @@
     </row>
     <row r="40" spans="1:13" ht="14.25" customHeight="1" thickBot="1">
       <c r="A40" s="113"/>
-      <c r="B40" s="280" t="s">
+      <c r="B40" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="280"/>
-      <c r="D40" s="280"/>
+      <c r="C40" s="235"/>
+      <c r="D40" s="235"/>
       <c r="E40" s="114"/>
       <c r="F40" s="124"/>
       <c r="G40" s="124"/>
@@ -12494,17 +12416,14 @@
     <row r="41" spans="1:13" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="L3:T3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:T4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
     <mergeCell ref="O5:T5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:E6"/>
@@ -12514,14 +12433,17 @@
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:T2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:T4"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F38:M38" xr:uid="{10C9E3CE-725B-4F12-9EDA-833D9294882B}">
@@ -12572,175 +12494,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="283" t="str">
+      <c r="B1" s="283"/>
+      <c r="C1" s="285" t="str">
         <f>FunctionList!E12</f>
         <v>FN02</v>
       </c>
-      <c r="D1" s="284"/>
+      <c r="D1" s="286"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D12</f>
         <v>Thiếp lập CSDL</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="282"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="284"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="285" t="s">
+      <c r="A2" s="287" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="286"/>
-      <c r="C2" s="287" t="s">
+      <c r="B2" s="288"/>
+      <c r="C2" s="289" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="288"/>
+      <c r="D2" s="290"/>
       <c r="E2" s="118"/>
-      <c r="F2" s="239" t="s">
+      <c r="F2" s="271" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="240"/>
-      <c r="H2" s="240"/>
-      <c r="I2" s="240"/>
-      <c r="J2" s="240"/>
-      <c r="K2" s="241"/>
-      <c r="L2" s="247" t="s">
+      <c r="G2" s="272"/>
+      <c r="H2" s="272"/>
+      <c r="I2" s="272"/>
+      <c r="J2" s="272"/>
+      <c r="K2" s="273"/>
+      <c r="L2" s="279" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="289"/>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="289"/>
-      <c r="R2" s="289"/>
-      <c r="S2" s="289"/>
-      <c r="T2" s="290"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="291"/>
+      <c r="R2" s="291"/>
+      <c r="S2" s="291"/>
+      <c r="T2" s="292"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="291" t="s">
+      <c r="A3" s="281" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="292"/>
-      <c r="C3" s="266">
+      <c r="B3" s="282"/>
+      <c r="C3" s="238">
         <v>100</v>
       </c>
-      <c r="D3" s="267"/>
+      <c r="D3" s="239"/>
       <c r="E3" s="65"/>
-      <c r="F3" s="268" t="s">
+      <c r="F3" s="240" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="269"/>
-      <c r="H3" s="269"/>
-      <c r="I3" s="269"/>
-      <c r="J3" s="269"/>
-      <c r="K3" s="270"/>
-      <c r="L3" s="271">
+      <c r="G3" s="241"/>
+      <c r="H3" s="241"/>
+      <c r="I3" s="241"/>
+      <c r="J3" s="241"/>
+      <c r="K3" s="242"/>
+      <c r="L3" s="243">
         <f xml:space="preserve"> IF(FunctionList!E6&lt;&gt;"N/A",SUM(C3*FunctionList!E6/1000,- O6),"N/A")</f>
         <v>5</v>
       </c>
-      <c r="M3" s="272"/>
-      <c r="N3" s="272"/>
-      <c r="O3" s="272"/>
-      <c r="P3" s="272"/>
-      <c r="Q3" s="272"/>
-      <c r="R3" s="272"/>
-      <c r="S3" s="272"/>
-      <c r="T3" s="273"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="244"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="245"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF($F$33:$HG$33,"P")</f>
         <v>5</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F33:HG33,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E32:HG32,"N")</f>
         <v>5</v>
@@ -12753,15 +12675,15 @@
         <f>COUNTIF($E$32:$HG$32,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HJ8)</f>
         <v>5</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1"/>
     <row r="8" spans="1:20" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -12908,10 +12830,10 @@
       <c r="A17" s="78"/>
       <c r="B17" s="79"/>
       <c r="C17" s="80"/>
-      <c r="D17" s="276" t="s">
+      <c r="D17" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="276"/>
+      <c r="E17" s="231"/>
       <c r="F17" s="110" t="s">
         <v>101</v>
       </c>
@@ -13142,11 +13064,11 @@
       <c r="A32" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="277" t="s">
+      <c r="B32" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="277"/>
-      <c r="D32" s="277"/>
+      <c r="C32" s="232"/>
+      <c r="D32" s="232"/>
       <c r="E32" s="107"/>
       <c r="F32" s="108" t="s">
         <v>53</v>
@@ -13166,11 +13088,11 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="95"/>
-      <c r="B33" s="278" t="s">
+      <c r="B33" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="278"/>
-      <c r="D33" s="278"/>
+      <c r="C33" s="233"/>
+      <c r="D33" s="233"/>
       <c r="E33" s="109"/>
       <c r="F33" s="110" t="s">
         <v>91</v>
@@ -13190,11 +13112,11 @@
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="95"/>
-      <c r="B34" s="279" t="s">
+      <c r="B34" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="279"/>
-      <c r="D34" s="279"/>
+      <c r="C34" s="234"/>
+      <c r="D34" s="234"/>
       <c r="E34" s="111"/>
       <c r="F34" s="112">
         <v>43468</v>
@@ -13214,11 +13136,11 @@
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1">
       <c r="A35" s="113"/>
-      <c r="B35" s="280" t="s">
+      <c r="B35" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="280"/>
-      <c r="D35" s="280"/>
+      <c r="C35" s="235"/>
+      <c r="D35" s="235"/>
       <c r="E35" s="114"/>
       <c r="F35" s="115"/>
       <c r="G35" s="115"/>
@@ -13229,17 +13151,14 @@
     <row r="36" spans="1:10" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:T2"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="O5:T5"/>
     <mergeCell ref="C4:T4"/>
@@ -13249,14 +13168,17 @@
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32:J32" xr:uid="{9F1C8E75-1B1D-45A0-92F5-75BABDDEE764}">
@@ -13279,8 +13201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B58F1-7BA3-45D5-8150-20CDE03D9739}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13307,43 +13229,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="281"/>
+      <c r="B1" s="283"/>
       <c r="C1" s="302" t="str">
         <f>FunctionList!E13</f>
         <v>FN03</v>
       </c>
-      <c r="D1" s="288"/>
+      <c r="D1" s="290"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D13</f>
         <v>Thêm mới tài khoản</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="236"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
       <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>65</v>
       </c>
@@ -13368,10 +13290,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -13399,82 +13321,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F51:HE51,"P")</f>
         <v>3</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F51:HE51,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E50:HE50,"N")</f>
         <v>3</v>
@@ -13487,15 +13409,15 @@
         <f>COUNTIF(E50:HE50,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HH8)</f>
         <v>3</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1"/>
     <row r="8" spans="1:21" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -13544,7 +13466,9 @@
       <c r="A11" s="78"/>
       <c r="B11" s="79"/>
       <c r="C11" s="80"/>
-      <c r="D11" s="81"/>
+      <c r="D11" s="81" t="s">
+        <v>297</v>
+      </c>
       <c r="E11" s="76"/>
       <c r="F11" s="110"/>
       <c r="G11" s="110"/>
@@ -14056,11 +13980,11 @@
       <c r="A50" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="277" t="s">
+      <c r="B50" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="277"/>
-      <c r="D50" s="277"/>
+      <c r="C50" s="232"/>
+      <c r="D50" s="232"/>
       <c r="E50" s="107"/>
       <c r="F50" s="108" t="s">
         <v>53</v>
@@ -14074,11 +13998,11 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="95"/>
-      <c r="B51" s="278" t="s">
+      <c r="B51" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="278"/>
-      <c r="D51" s="278"/>
+      <c r="C51" s="233"/>
+      <c r="D51" s="233"/>
       <c r="E51" s="109"/>
       <c r="F51" s="110" t="s">
         <v>91</v>
@@ -14092,11 +14016,11 @@
     </row>
     <row r="52" spans="1:8" ht="13.5" customHeight="1">
       <c r="A52" s="95"/>
-      <c r="B52" s="279" t="s">
+      <c r="B52" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="279"/>
-      <c r="D52" s="279"/>
+      <c r="C52" s="234"/>
+      <c r="D52" s="234"/>
       <c r="E52" s="111"/>
       <c r="F52" s="112">
         <v>43468</v>
@@ -14110,11 +14034,11 @@
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1">
       <c r="A53" s="113"/>
-      <c r="B53" s="280" t="s">
+      <c r="B53" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="280"/>
-      <c r="D53" s="280"/>
+      <c r="C53" s="235"/>
+      <c r="D53" s="235"/>
       <c r="E53" s="114"/>
       <c r="F53" s="115"/>
       <c r="G53" s="115"/>
@@ -14123,19 +14047,6 @@
     <row r="54" spans="1:8" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="A4:B4"/>
@@ -14150,6 +14061,19 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <dataValidations count="3">
@@ -14200,43 +14124,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="245" t="str">
+      <c r="B1" s="264"/>
+      <c r="C1" s="277" t="str">
         <f>FunctionList!E14</f>
         <v>FN04</v>
       </c>
-      <c r="D1" s="246"/>
+      <c r="D1" s="278"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D14</f>
         <v>Sửa tài khoản</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="236"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
       <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -14263,10 +14187,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -14294,82 +14218,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F44:HJ44,"P")</f>
         <v>0</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F44:HJ44,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E43:HJ43,"N")</f>
         <v>0</v>
@@ -14382,15 +14306,15 @@
         <f>COUNTIF(E43:HJ43,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HM8)</f>
         <v>9</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1"/>
     <row r="8" spans="1:21" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -14609,10 +14533,10 @@
       <c r="A18" s="78"/>
       <c r="B18" s="79"/>
       <c r="C18" s="80"/>
-      <c r="D18" s="276" t="s">
+      <c r="D18" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="276"/>
+      <c r="E18" s="231"/>
       <c r="F18" s="110" t="s">
         <v>101</v>
       </c>
@@ -14698,10 +14622,10 @@
       <c r="A22" s="78"/>
       <c r="B22" s="79"/>
       <c r="C22" s="80"/>
-      <c r="D22" s="276" t="s">
+      <c r="D22" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="276"/>
+      <c r="E22" s="231"/>
       <c r="F22" s="110" t="s">
         <v>101</v>
       </c>
@@ -14768,10 +14692,10 @@
       <c r="A25" s="78"/>
       <c r="B25" s="79"/>
       <c r="C25" s="80"/>
-      <c r="D25" s="276" t="s">
+      <c r="D25" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="276"/>
+      <c r="E25" s="231"/>
       <c r="F25" s="110" t="s">
         <v>101</v>
       </c>
@@ -14839,10 +14763,10 @@
       <c r="A28" s="78"/>
       <c r="B28" s="136"/>
       <c r="C28" s="137"/>
-      <c r="D28" s="276" t="s">
+      <c r="D28" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="276"/>
+      <c r="E28" s="231"/>
       <c r="F28" s="128" t="s">
         <v>101</v>
       </c>
@@ -14873,10 +14797,10 @@
       <c r="A29" s="78"/>
       <c r="B29" s="132"/>
       <c r="C29" s="133"/>
-      <c r="D29" s="276" t="s">
+      <c r="D29" s="231" t="s">
         <v>226</v>
       </c>
-      <c r="E29" s="276"/>
+      <c r="E29" s="231"/>
       <c r="F29" s="128"/>
       <c r="G29" s="128"/>
       <c r="H29" s="128"/>
@@ -15310,15 +15234,13 @@
     <row r="48" spans="1:14" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
@@ -15335,13 +15257,15 @@
     <mergeCell ref="L1:T1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <dataValidations count="3">
@@ -15393,42 +15317,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="264"/>
       <c r="C1" s="302" t="str">
         <f>FunctionList!E16</f>
         <v>FN06</v>
       </c>
-      <c r="D1" s="288"/>
+      <c r="D1" s="290"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266" t="str">
         <f>FunctionList!D16</f>
         <v>Kích hoạt tài khoản</v>
       </c>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="235"/>
-      <c r="S1" s="235"/>
-      <c r="T1" s="282"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="284"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="299" t="s">
         <v>3</v>
       </c>
@@ -15453,10 +15377,10 @@
       <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="303">
         <v>100</v>
       </c>
@@ -15484,82 +15408,82 @@
       <c r="T3" s="298"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="263"/>
-      <c r="L5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
+      <c r="K5" s="262"/>
+      <c r="L5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="249" t="s">
+      <c r="M5" s="249"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="250"/>
-      <c r="S5" s="250"/>
-      <c r="T5" s="251"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="250"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F43:HF43,"P")</f>
         <v>5</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F43:HF43,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(O6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="66">
         <f>COUNTIF(E42:HF42,"N")</f>
         <v>5</v>
@@ -15572,15 +15496,15 @@
         <f>COUNTIF(E42:HF42,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="257">
+      <c r="O6" s="256">
         <f>COUNTA(E8:HI8)</f>
         <v>5</v>
       </c>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="255"/>
-      <c r="S6" s="255"/>
-      <c r="T6" s="258"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="254"/>
+      <c r="S6" s="254"/>
+      <c r="T6" s="257"/>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1"/>
     <row r="8" spans="1:20" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -15729,10 +15653,10 @@
       <c r="A17" s="78"/>
       <c r="B17" s="79"/>
       <c r="C17" s="80"/>
-      <c r="D17" s="276" t="s">
+      <c r="D17" s="231" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="276"/>
+      <c r="E17" s="231"/>
       <c r="F17" s="127" t="s">
         <v>101</v>
       </c>
@@ -16129,11 +16053,11 @@
       <c r="A42" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="277" t="s">
+      <c r="B42" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="277"/>
-      <c r="D42" s="277"/>
+      <c r="C42" s="232"/>
+      <c r="D42" s="232"/>
       <c r="E42" s="107"/>
       <c r="F42" s="108" t="s">
         <v>53</v>
@@ -16153,11 +16077,11 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="95"/>
-      <c r="B43" s="278" t="s">
+      <c r="B43" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="278"/>
-      <c r="D43" s="278"/>
+      <c r="C43" s="233"/>
+      <c r="D43" s="233"/>
       <c r="E43" s="109"/>
       <c r="F43" s="110" t="s">
         <v>91</v>
@@ -16177,11 +16101,11 @@
     </row>
     <row r="44" spans="1:10" ht="13.5" customHeight="1">
       <c r="A44" s="95"/>
-      <c r="B44" s="279" t="s">
+      <c r="B44" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="279"/>
-      <c r="D44" s="279"/>
+      <c r="C44" s="234"/>
+      <c r="D44" s="234"/>
       <c r="E44" s="111"/>
       <c r="F44" s="112">
         <v>43468</v>
@@ -16201,11 +16125,11 @@
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1">
       <c r="A45" s="113"/>
-      <c r="B45" s="280" t="s">
+      <c r="B45" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="280"/>
-      <c r="D45" s="280"/>
+      <c r="C45" s="235"/>
+      <c r="D45" s="235"/>
       <c r="E45" s="114"/>
       <c r="F45" s="115"/>
       <c r="G45" s="115"/>
@@ -16216,11 +16140,13 @@
     <row r="46" spans="1:10" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="O6:T6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
@@ -16237,13 +16163,11 @@
     <mergeCell ref="L1:T1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <dataValidations count="3">
@@ -16292,40 +16216,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="263" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="283" t="str">
+      <c r="B1" s="264"/>
+      <c r="C1" s="285" t="str">
         <f>FunctionList!E15</f>
         <v>FN05</v>
       </c>
-      <c r="D1" s="284"/>
+      <c r="D1" s="286"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="233" t="s">
+      <c r="F1" s="265" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="234" t="str">
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="266" t="str">
         <f>FunctionList!D15</f>
         <v>Tìm kiếm tài khoản</v>
       </c>
-      <c r="K1" s="235"/>
-      <c r="L1" s="235"/>
-      <c r="M1" s="235"/>
-      <c r="N1" s="235"/>
-      <c r="O1" s="235"/>
-      <c r="P1" s="235"/>
-      <c r="Q1" s="235"/>
-      <c r="R1" s="282"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="284"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="264" t="s">
+      <c r="A2" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="265"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="317" t="s">
         <v>3</v>
       </c>
@@ -16350,14 +16274,14 @@
       <c r="R2" s="64"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="264" t="s">
+      <c r="A3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="265"/>
-      <c r="C3" s="266">
+      <c r="B3" s="237"/>
+      <c r="C3" s="238">
         <v>100</v>
       </c>
-      <c r="D3" s="267"/>
+      <c r="D3" s="239"/>
       <c r="E3" s="117"/>
       <c r="F3" s="293" t="s">
         <v>68</v>
@@ -16379,76 +16303,76 @@
       <c r="R3" s="298"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="265"/>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="274"/>
-      <c r="K4" s="274"/>
-      <c r="L4" s="274"/>
-      <c r="M4" s="274"/>
-      <c r="N4" s="274"/>
-      <c r="O4" s="274"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="246"/>
+      <c r="K4" s="246"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="246"/>
+      <c r="O4" s="246"/>
+      <c r="P4" s="246"/>
+      <c r="Q4" s="246"/>
+      <c r="R4" s="246"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="260"/>
-      <c r="C5" s="261" t="s">
+      <c r="B5" s="259"/>
+      <c r="C5" s="260" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="261" t="s">
+      <c r="D5" s="249"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="260" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="263"/>
-      <c r="J5" s="250" t="s">
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="262"/>
+      <c r="J5" s="249" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="250"/>
-      <c r="L5" s="250"/>
-      <c r="M5" s="249" t="s">
+      <c r="K5" s="249"/>
+      <c r="L5" s="249"/>
+      <c r="M5" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="250"/>
-      <c r="O5" s="250"/>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="251"/>
+      <c r="N5" s="249"/>
+      <c r="O5" s="249"/>
+      <c r="P5" s="249"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="250"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1">
-      <c r="A6" s="252">
+      <c r="A6" s="251">
         <f>COUNTIF(F29:HD29,"P")</f>
         <v>2</v>
       </c>
-      <c r="B6" s="253"/>
-      <c r="C6" s="254">
+      <c r="B6" s="252"/>
+      <c r="C6" s="253">
         <f>COUNTIF(F29:HD29,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="255"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="254">
+      <c r="D6" s="254"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="253">
         <f>SUM(M6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="256"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="255"/>
       <c r="J6" s="66">
         <f>COUNTIF(E28:HD28,"N")</f>
         <v>2</v>
@@ -16461,15 +16385,15 @@
         <f>COUNTIF(E28:HD28,"B")</f>
         <v>0</v>
       </c>
-      <c r="M6" s="257">
+      <c r="M6" s="256">
         <f>COUNTA(E8:HG8)</f>
         <v>2</v>
       </c>
-      <c r="N6" s="255"/>
-      <c r="O6" s="255"/>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
-      <c r="R6" s="258"/>
+      <c r="N6" s="254"/>
+      <c r="O6" s="254"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="257"/>
     </row>
     <row r="7" spans="1:18" ht="15" thickBot="1"/>
     <row r="8" spans="1:18" ht="37.200000000000003" thickTop="1" thickBot="1">
@@ -16700,11 +16624,11 @@
       <c r="A28" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="277" t="s">
+      <c r="B28" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="277"/>
-      <c r="D28" s="277"/>
+      <c r="C28" s="232"/>
+      <c r="D28" s="232"/>
       <c r="E28" s="107"/>
       <c r="F28" s="108" t="s">
         <v>53</v>
@@ -16715,11 +16639,11 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="95"/>
-      <c r="B29" s="278" t="s">
+      <c r="B29" s="233" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="278"/>
-      <c r="D29" s="278"/>
+      <c r="C29" s="233"/>
+      <c r="D29" s="233"/>
       <c r="E29" s="109"/>
       <c r="F29" s="110" t="s">
         <v>91</v>
@@ -16730,11 +16654,11 @@
     </row>
     <row r="30" spans="1:7" ht="13.5" customHeight="1">
       <c r="A30" s="95"/>
-      <c r="B30" s="279" t="s">
+      <c r="B30" s="234" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="279"/>
-      <c r="D30" s="279"/>
+      <c r="C30" s="234"/>
+      <c r="D30" s="234"/>
       <c r="E30" s="111"/>
       <c r="F30" s="112">
         <v>43468</v>
@@ -16745,11 +16669,11 @@
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1">
       <c r="A31" s="113"/>
-      <c r="B31" s="280" t="s">
+      <c r="B31" s="235" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="280"/>
-      <c r="D31" s="280"/>
+      <c r="C31" s="235"/>
+      <c r="D31" s="235"/>
       <c r="E31" s="114"/>
       <c r="F31" s="115"/>
       <c r="G31" s="115"/>
@@ -16757,12 +16681,16 @@
     <row r="32" spans="1:7" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="M5:R5"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
@@ -16770,20 +16698,16 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="M6:R6"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L2"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="J5:L5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:R3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:G28" xr:uid="{E516B88F-32AA-4A5A-9BBC-7EC121A05672}">

</xml_diff>